<commit_message>
raw data work and code updates
</commit_message>
<xml_diff>
--- a/raw_ts_data/fd/fd12_ts2.xlsx
+++ b/raw_ts_data/fd/fd12_ts2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncw02\Downloads\IGEA\raw_ts_data\fd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9004E96-A502-471E-945B-0F2453CA0A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DB12F5-1CBB-4F94-B032-B18FC1E21F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E68C062C-7D11-714A-B9EB-02BD676A21BD}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2834" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2836" uniqueCount="94">
   <si>
     <t>Reach</t>
   </si>
@@ -314,6 +314,12 @@
   <si>
     <t>TP09</t>
   </si>
+  <si>
+    <t>ERRORCODE</t>
+  </si>
+  <si>
+    <t>ADJUSTMENT</t>
+  </si>
 </sst>
 </file>
 
@@ -398,7 +404,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -414,10 +420,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,13 +747,13 @@
   <dimension ref="A1:AC1381"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <pane ySplit="1" topLeftCell="A426" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F436" sqref="F436"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.21875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="75" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -764,11 +773,15 @@
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -809,6 +822,9 @@
       <c r="G2" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="H2" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
@@ -829,6 +845,9 @@
       <c r="G3" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="H3" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
@@ -849,6 +868,9 @@
       <c r="G4" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="H4" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
@@ -869,6 +891,9 @@
       <c r="G5" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="H5" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
@@ -889,6 +914,9 @@
       <c r="G6" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="H6" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
@@ -909,6 +937,9 @@
       <c r="G7" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="H7" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
@@ -1916,7 +1947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B65" s="2" t="s">
         <v>5</v>
       </c>
@@ -1933,7 +1964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B66" s="2" t="s">
         <v>5</v>
       </c>
@@ -1950,7 +1981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B67" s="2" t="s">
         <v>5</v>
       </c>
@@ -1967,7 +1998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B68" s="2" t="s">
         <v>5</v>
       </c>
@@ -1984,7 +2015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B69" s="2" t="s">
         <v>5</v>
       </c>
@@ -2001,7 +2032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B70" s="2" t="s">
         <v>5</v>
       </c>
@@ -2020,8 +2051,11 @@
       <c r="G70" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="71" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H70" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B71" s="2" t="s">
         <v>5</v>
       </c>
@@ -2040,8 +2074,11 @@
       <c r="G71" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="72" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H71" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B72" s="2" t="s">
         <v>5</v>
       </c>
@@ -2060,8 +2097,11 @@
       <c r="G72" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="73" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H72" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B73" s="2" t="s">
         <v>5</v>
       </c>
@@ -2080,8 +2120,11 @@
       <c r="G73" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="74" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H73" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B74" s="2" t="s">
         <v>5</v>
       </c>
@@ -2100,8 +2143,11 @@
       <c r="G74" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="75" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H74" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B75" s="2" t="s">
         <v>5</v>
       </c>
@@ -2120,8 +2166,11 @@
       <c r="G75" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="76" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H75" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B76" s="2" t="s">
         <v>5</v>
       </c>
@@ -2140,8 +2189,11 @@
       <c r="G76" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="77" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H76" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B77" s="2" t="s">
         <v>5</v>
       </c>
@@ -2158,7 +2210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B78" s="2" t="s">
         <v>5</v>
       </c>
@@ -2175,7 +2227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B79" s="2" t="s">
         <v>5</v>
       </c>
@@ -2192,7 +2244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B80" s="2" t="s">
         <v>5</v>
       </c>
@@ -2277,7 +2329,7 @@
       <c r="F84" s="6">
         <v>1</v>
       </c>
-      <c r="G84" s="6"/>
+      <c r="G84" s="13"/>
       <c r="H84" s="6"/>
       <c r="I84" s="6"/>
       <c r="J84" s="6"/>
@@ -2505,7 +2557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B97" s="2" t="s">
         <v>88</v>
       </c>
@@ -2522,7 +2574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B98" s="2" t="s">
         <v>88</v>
       </c>
@@ -2538,11 +2590,14 @@
       <c r="F98" s="2">
         <v>3</v>
       </c>
-      <c r="G98" s="2" t="s">
+      <c r="G98" s="14" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="99" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H98" s="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B99" s="2" t="s">
         <v>88</v>
       </c>
@@ -2559,7 +2614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B100" s="2" t="s">
         <v>88</v>
       </c>
@@ -2576,7 +2631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B101" s="2" t="s">
         <v>88</v>
       </c>
@@ -2593,7 +2648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B102" s="2" t="s">
         <v>88</v>
       </c>
@@ -2609,11 +2664,14 @@
       <c r="F102" s="2">
         <v>4</v>
       </c>
-      <c r="G102" s="2" t="s">
+      <c r="G102" s="14" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="103" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H102" s="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B103" s="2" t="s">
         <v>88</v>
       </c>
@@ -2630,7 +2688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B104" s="2" t="s">
         <v>88</v>
       </c>
@@ -2647,7 +2705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B105" s="2" t="s">
         <v>88</v>
       </c>
@@ -2664,7 +2722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B106" s="2" t="s">
         <v>88</v>
       </c>
@@ -2681,7 +2739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B107" s="2" t="s">
         <v>88</v>
       </c>
@@ -2698,7 +2756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B108" s="2" t="s">
         <v>88</v>
       </c>
@@ -2715,7 +2773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B109" s="2" t="s">
         <v>88</v>
       </c>
@@ -2731,11 +2789,11 @@
       <c r="F109" s="2">
         <v>1</v>
       </c>
-      <c r="G109" s="11" t="s">
+      <c r="G109" s="15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="110" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B110" s="2" t="s">
         <v>88</v>
       </c>
@@ -2751,9 +2809,9 @@
       <c r="F110" s="2">
         <v>1</v>
       </c>
-      <c r="G110" s="12"/>
-    </row>
-    <row r="111" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="G110" s="16"/>
+    </row>
+    <row r="111" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B111" s="2" t="s">
         <v>88</v>
       </c>
@@ -2770,7 +2828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B112" s="2" t="s">
         <v>88</v>
       </c>
@@ -3007,7 +3065,7 @@
       <c r="F125" s="2">
         <v>1</v>
       </c>
-      <c r="G125" s="2" t="s">
+      <c r="G125" s="14" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4369,7 +4427,7 @@
       <c r="F205" s="6">
         <v>1</v>
       </c>
-      <c r="G205" s="6"/>
+      <c r="G205" s="13"/>
       <c r="H205" s="6"/>
       <c r="I205" s="6"/>
       <c r="J205" s="6"/>
@@ -4698,7 +4756,7 @@
       <c r="F223" s="2">
         <v>1</v>
       </c>
-      <c r="G223" s="2" t="s">
+      <c r="G223" s="14" t="s">
         <v>42</v>
       </c>
     </row>
@@ -4973,7 +5031,7 @@
       <c r="F239" s="2">
         <v>1</v>
       </c>
-      <c r="G239" s="2" t="s">
+      <c r="G239" s="14" t="s">
         <v>43</v>
       </c>
     </row>
@@ -5588,7 +5646,7 @@
       <c r="F275" s="2">
         <v>1</v>
       </c>
-      <c r="G275" s="2" t="s">
+      <c r="G275" s="14" t="s">
         <v>44</v>
       </c>
     </row>
@@ -6272,7 +6330,7 @@
       <c r="F315" s="6">
         <v>1</v>
       </c>
-      <c r="G315" s="6"/>
+      <c r="G315" s="13"/>
       <c r="H315" s="6"/>
       <c r="I315" s="6"/>
       <c r="J315" s="6"/>
@@ -7191,7 +7249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="369" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="369" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B369" s="2" t="s">
         <v>87</v>
       </c>
@@ -7208,7 +7266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="370" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="370" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B370" s="2" t="s">
         <v>87</v>
       </c>
@@ -7225,7 +7283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="371" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="371" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B371" s="2" t="s">
         <v>87</v>
       </c>
@@ -7242,7 +7300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="372" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="372" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B372" s="2" t="s">
         <v>87</v>
       </c>
@@ -7259,7 +7317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="373" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="373" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B373" s="2" t="s">
         <v>87</v>
       </c>
@@ -7276,7 +7334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="374" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="374" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B374" s="2" t="s">
         <v>87</v>
       </c>
@@ -7293,7 +7351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="375" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="375" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B375" s="2" t="s">
         <v>87</v>
       </c>
@@ -7309,11 +7367,14 @@
       <c r="F375" s="2">
         <v>1</v>
       </c>
-      <c r="G375" s="2" t="s">
+      <c r="G375" s="14" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="376" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H375" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="376" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B376" s="2" t="s">
         <v>87</v>
       </c>
@@ -7329,11 +7390,12 @@
       <c r="F376" s="2">
         <v>1</v>
       </c>
-      <c r="G376" s="2" t="s">
+      <c r="G376" s="14" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="377" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H376" s="14"/>
+    </row>
+    <row r="377" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B377" s="2" t="s">
         <v>87</v>
       </c>
@@ -7350,7 +7412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="378" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="378" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B378" s="2" t="s">
         <v>87</v>
       </c>
@@ -7367,7 +7429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="379" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="379" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B379" s="2" t="s">
         <v>87</v>
       </c>
@@ -7384,7 +7446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="380" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="380" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B380" s="2" t="s">
         <v>87</v>
       </c>
@@ -7401,7 +7463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="381" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="381" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B381" s="2" t="s">
         <v>87</v>
       </c>
@@ -7418,7 +7480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="382" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="382" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B382" s="2" t="s">
         <v>87</v>
       </c>
@@ -7435,7 +7497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="383" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="383" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B383" s="2" t="s">
         <v>87</v>
       </c>
@@ -7452,7 +7514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="384" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="384" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B384" s="2" t="s">
         <v>87</v>
       </c>
@@ -7701,7 +7763,7 @@
         <v>183</v>
       </c>
       <c r="E398" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F398" s="2">
         <v>1</v>
@@ -7718,7 +7780,7 @@
         <v>184</v>
       </c>
       <c r="E399" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F399" s="2">
         <v>1</v>
@@ -7735,7 +7797,7 @@
         <v>185</v>
       </c>
       <c r="E400" s="8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F400" s="2">
         <v>1</v>
@@ -7752,7 +7814,7 @@
         <v>186</v>
       </c>
       <c r="E401" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F401" s="2">
         <v>1</v>
@@ -7769,7 +7831,7 @@
         <v>187</v>
       </c>
       <c r="E402" s="8" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F402" s="2">
         <v>1</v>
@@ -7786,7 +7848,7 @@
         <v>188</v>
       </c>
       <c r="E403" s="8" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F403" s="2">
         <v>1</v>
@@ -7803,7 +7865,7 @@
         <v>189</v>
       </c>
       <c r="E404" s="8" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="F404" s="2">
         <v>1</v>
@@ -7820,7 +7882,7 @@
         <v>190</v>
       </c>
       <c r="E405" s="8" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="F405" s="2">
         <v>1</v>
@@ -7837,7 +7899,7 @@
         <v>191</v>
       </c>
       <c r="E406" s="8" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="F406" s="2">
         <v>1</v>
@@ -7854,7 +7916,7 @@
         <v>192</v>
       </c>
       <c r="E407" s="8" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="F407" s="2">
         <v>1</v>
@@ -7871,7 +7933,7 @@
         <v>193</v>
       </c>
       <c r="E408" s="8" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F408" s="2">
         <v>1</v>
@@ -7888,7 +7950,7 @@
         <v>194</v>
       </c>
       <c r="E409" s="8" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F409" s="2">
         <v>1</v>
@@ -7905,7 +7967,7 @@
         <v>195</v>
       </c>
       <c r="E410" s="8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F410" s="2">
         <v>1</v>
@@ -7922,7 +7984,7 @@
         <v>196</v>
       </c>
       <c r="E411" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F411" s="2">
         <v>1</v>
@@ -7939,7 +8001,7 @@
         <v>197</v>
       </c>
       <c r="E412" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F412" s="2">
         <v>1</v>
@@ -7956,7 +8018,7 @@
         <v>198</v>
       </c>
       <c r="E413" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F413" s="2">
         <v>1</v>
@@ -7973,7 +8035,7 @@
         <v>199</v>
       </c>
       <c r="E414" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F414" s="2">
         <v>1</v>
@@ -7990,7 +8052,7 @@
         <v>200</v>
       </c>
       <c r="E415" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F415" s="2">
         <v>1</v>
@@ -8007,7 +8069,7 @@
         <v>201</v>
       </c>
       <c r="E416" s="8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F416" s="2">
         <v>1</v>
@@ -8024,7 +8086,7 @@
         <v>202</v>
       </c>
       <c r="E417" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F417" s="2">
         <v>1</v>
@@ -8041,7 +8103,7 @@
         <v>203</v>
       </c>
       <c r="E418" s="8" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F418" s="2">
         <v>1</v>
@@ -8058,7 +8120,7 @@
         <v>204</v>
       </c>
       <c r="E419" s="8" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F419" s="2">
         <v>1</v>
@@ -8075,7 +8137,7 @@
         <v>205</v>
       </c>
       <c r="E420" s="8" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="F420" s="2">
         <v>1</v>
@@ -8092,7 +8154,7 @@
         <v>206</v>
       </c>
       <c r="E421" s="8" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="F421" s="2">
         <v>1</v>
@@ -8109,7 +8171,7 @@
         <v>207</v>
       </c>
       <c r="E422" s="8" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="F422" s="2">
         <v>1</v>
@@ -8126,12 +8188,12 @@
         <v>208</v>
       </c>
       <c r="E423" s="8" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="F423" s="2">
         <v>1</v>
       </c>
-      <c r="G423" s="2" t="s">
+      <c r="G423" s="14" t="s">
         <v>48</v>
       </c>
     </row>
@@ -8146,7 +8208,7 @@
         <v>209</v>
       </c>
       <c r="E424" s="8" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F424" s="2">
         <v>1</v>
@@ -8163,7 +8225,7 @@
         <v>210</v>
       </c>
       <c r="E425" s="8" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F425" s="2">
         <v>1</v>
@@ -8180,7 +8242,7 @@
         <v>211</v>
       </c>
       <c r="E426" s="8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F426" s="2">
         <v>1</v>
@@ -8197,7 +8259,7 @@
         <v>212</v>
       </c>
       <c r="E427" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F427" s="2">
         <v>1</v>
@@ -8214,7 +8276,7 @@
         <v>213</v>
       </c>
       <c r="E428" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F428" s="2">
         <v>1</v>
@@ -8231,7 +8293,7 @@
         <v>214</v>
       </c>
       <c r="E429" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F429" s="2">
         <v>1</v>
@@ -8248,7 +8310,7 @@
         <v>215</v>
       </c>
       <c r="E430" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F430" s="2">
         <v>1</v>
@@ -8265,7 +8327,7 @@
         <v>216</v>
       </c>
       <c r="E431" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F431" s="2">
         <v>1</v>
@@ -8282,7 +8344,7 @@
         <v>217</v>
       </c>
       <c r="E432" s="8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F432" s="2">
         <v>1</v>
@@ -8299,7 +8361,7 @@
         <v>218</v>
       </c>
       <c r="E433" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F433" s="2">
         <v>1</v>
@@ -8316,7 +8378,7 @@
         <v>219</v>
       </c>
       <c r="E434" s="8" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F434" s="2">
         <v>1</v>
@@ -8333,7 +8395,7 @@
         <v>220</v>
       </c>
       <c r="E435" s="8" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F435" s="2">
         <v>1</v>
@@ -8350,7 +8412,7 @@
         <v>221</v>
       </c>
       <c r="E436" s="8" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="F436" s="2">
         <v>1</v>
@@ -8367,7 +8429,7 @@
         <v>222</v>
       </c>
       <c r="E437" s="8" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="F437" s="2">
         <v>1</v>
@@ -8386,7 +8448,7 @@
         <v>41</v>
       </c>
       <c r="F438" s="6"/>
-      <c r="G438" s="6"/>
+      <c r="G438" s="13"/>
       <c r="H438" s="6"/>
       <c r="I438" s="6"/>
       <c r="J438" s="6"/>
@@ -9083,7 +9145,7 @@
       <c r="F478" s="2">
         <v>1</v>
       </c>
-      <c r="G478" s="2" t="s">
+      <c r="G478" s="14" t="s">
         <v>50</v>
       </c>
     </row>
@@ -9460,7 +9522,7 @@
       <c r="F500" s="2">
         <v>1</v>
       </c>
-      <c r="G500" s="2" t="s">
+      <c r="G500" s="14" t="s">
         <v>52</v>
       </c>
     </row>
@@ -9480,7 +9542,7 @@
       <c r="F501" s="2">
         <v>1</v>
       </c>
-      <c r="G501" s="2" t="s">
+      <c r="G501" s="14" t="s">
         <v>52</v>
       </c>
     </row>
@@ -9500,7 +9562,7 @@
       <c r="F502" s="2">
         <v>1</v>
       </c>
-      <c r="G502" s="2" t="s">
+      <c r="G502" s="14" t="s">
         <v>52</v>
       </c>
     </row>
@@ -9520,7 +9582,7 @@
       <c r="F503" s="2">
         <v>1</v>
       </c>
-      <c r="G503" s="2" t="s">
+      <c r="G503" s="14" t="s">
         <v>52</v>
       </c>
     </row>
@@ -9537,7 +9599,7 @@
         <v>41</v>
       </c>
       <c r="F504" s="6"/>
-      <c r="G504" s="6"/>
+      <c r="G504" s="13"/>
       <c r="H504" s="6"/>
       <c r="I504" s="6"/>
       <c r="J504" s="6"/>
@@ -9945,7 +10007,7 @@
       <c r="F527" s="2">
         <v>1</v>
       </c>
-      <c r="G527" s="2" t="s">
+      <c r="G527" s="14" t="s">
         <v>55</v>
       </c>
     </row>
@@ -10676,7 +10738,7 @@
         <v>41</v>
       </c>
       <c r="F570" s="6"/>
-      <c r="G570" s="6"/>
+      <c r="G570" s="13"/>
       <c r="H570" s="6"/>
       <c r="I570" s="6"/>
       <c r="J570" s="6"/>
@@ -11618,7 +11680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="625" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="625" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B625" s="2" t="s">
         <v>86</v>
       </c>
@@ -11635,7 +11697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="626" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="626" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B626" s="2" t="s">
         <v>86</v>
       </c>
@@ -11652,7 +11714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="627" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="627" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B627" s="2" t="s">
         <v>86</v>
       </c>
@@ -11669,7 +11731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="628" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="628" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B628" s="2" t="s">
         <v>86</v>
       </c>
@@ -11686,7 +11748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="629" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="629" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B629" s="2" t="s">
         <v>86</v>
       </c>
@@ -11703,7 +11765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="630" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="630" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B630" s="2" t="s">
         <v>86</v>
       </c>
@@ -11720,7 +11782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="631" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="631" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B631" s="2" t="s">
         <v>86</v>
       </c>
@@ -11737,7 +11799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="632" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="632" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B632" s="2" t="s">
         <v>86</v>
       </c>
@@ -11754,7 +11816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="633" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="633" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B633" s="2" t="s">
         <v>86</v>
       </c>
@@ -11771,7 +11833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="634" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="634" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B634" s="2" t="s">
         <v>86</v>
       </c>
@@ -11788,7 +11850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="635" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="635" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B635" s="2" t="s">
         <v>86</v>
       </c>
@@ -11805,7 +11867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="636" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="636" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B636" s="2" t="s">
         <v>86</v>
       </c>
@@ -11818,11 +11880,14 @@
       <c r="F636" s="2">
         <v>1</v>
       </c>
-      <c r="G636" s="2" t="s">
+      <c r="G636" s="14" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="637" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H636" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="637" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B637" s="2" t="s">
         <v>86</v>
       </c>
@@ -11839,7 +11904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="638" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="638" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B638" s="2" t="s">
         <v>86</v>
       </c>
@@ -11856,7 +11921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="639" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="639" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B639" s="2" t="s">
         <v>86</v>
       </c>
@@ -11873,7 +11938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="640" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="640" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B640" s="2" t="s">
         <v>86</v>
       </c>
@@ -14179,7 +14244,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="785" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="785" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B785" s="2" t="s">
         <v>91</v>
       </c>
@@ -14193,7 +14258,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="786" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="786" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B786" s="2" t="s">
         <v>91</v>
       </c>
@@ -14207,7 +14272,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="787" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="787" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B787" s="2" t="s">
         <v>91</v>
       </c>
@@ -14221,7 +14286,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="788" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="788" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B788" s="2" t="s">
         <v>91</v>
       </c>
@@ -14235,7 +14300,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="789" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="789" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B789" s="2" t="s">
         <v>91</v>
       </c>
@@ -14249,7 +14314,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="790" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="790" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B790" s="2" t="s">
         <v>91</v>
       </c>
@@ -14263,7 +14328,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="791" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="791" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B791" s="2" t="s">
         <v>91</v>
       </c>
@@ -14277,7 +14342,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="792" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="792" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B792" s="2" t="s">
         <v>91</v>
       </c>
@@ -14291,7 +14356,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="793" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="793" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B793" s="2" t="s">
         <v>91</v>
       </c>
@@ -14305,7 +14370,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="794" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="794" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B794" s="2" t="s">
         <v>91</v>
       </c>
@@ -14319,7 +14384,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="795" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="795" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B795" s="2" t="s">
         <v>91</v>
       </c>
@@ -14333,7 +14398,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="796" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="796" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B796" s="2" t="s">
         <v>91</v>
       </c>
@@ -14347,7 +14412,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="797" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="797" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B797" s="2" t="s">
         <v>91</v>
       </c>
@@ -14357,11 +14422,14 @@
       <c r="D797" s="2">
         <v>166</v>
       </c>
-      <c r="G797" s="2" t="s">
+      <c r="G797" s="14" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="798" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H797">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="798" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B798" s="2" t="s">
         <v>91</v>
       </c>
@@ -14371,11 +14439,14 @@
       <c r="D798" s="2">
         <v>167</v>
       </c>
-      <c r="G798" s="2" t="s">
+      <c r="G798" s="14" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="799" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H798">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="799" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B799" s="2" t="s">
         <v>91</v>
       </c>
@@ -14389,7 +14460,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="800" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="800" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B800" s="2" t="s">
         <v>91</v>
       </c>
@@ -14848,7 +14919,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="833" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="833" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B833" s="2" t="s">
         <v>59</v>
       </c>
@@ -14862,7 +14933,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="834" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="834" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B834" s="2" t="s">
         <v>59</v>
       </c>
@@ -14876,7 +14947,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="835" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="835" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B835" s="2" t="s">
         <v>59</v>
       </c>
@@ -14890,7 +14961,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="836" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="836" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B836" s="2" t="s">
         <v>59</v>
       </c>
@@ -14904,7 +14975,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="837" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="837" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B837" s="2" t="s">
         <v>59</v>
       </c>
@@ -14918,7 +14989,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="838" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="838" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B838" s="2" t="s">
         <v>59</v>
       </c>
@@ -14932,7 +15003,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="839" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="839" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B839" s="2" t="s">
         <v>59</v>
       </c>
@@ -14945,11 +15016,14 @@
       <c r="E839" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G839" s="2" t="s">
+      <c r="G839" s="14" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="840" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H839">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="840" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B840" s="2" t="s">
         <v>59</v>
       </c>
@@ -14962,11 +15036,14 @@
       <c r="E840" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G840" s="2" t="s">
+      <c r="G840" s="14" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="841" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H840">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="841" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B841" s="2" t="s">
         <v>59</v>
       </c>
@@ -14979,11 +15056,14 @@
       <c r="E841" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G841" s="2" t="s">
+      <c r="G841" s="14" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="842" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H841">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="842" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B842" s="2" t="s">
         <v>59</v>
       </c>
@@ -14996,11 +15076,14 @@
       <c r="E842" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G842" s="2" t="s">
+      <c r="G842" s="14" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="843" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H842">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="843" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B843" s="2" t="s">
         <v>59</v>
       </c>
@@ -15013,11 +15096,14 @@
       <c r="E843" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G843" s="2" t="s">
+      <c r="G843" s="14" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="844" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H843">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="844" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B844" s="2" t="s">
         <v>59</v>
       </c>
@@ -15030,11 +15116,14 @@
       <c r="E844" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G844" s="2" t="s">
+      <c r="G844" s="14" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="845" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H844">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="845" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B845" s="2" t="s">
         <v>59</v>
       </c>
@@ -15048,7 +15137,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="846" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="846" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B846" s="2" t="s">
         <v>59</v>
       </c>
@@ -15062,7 +15151,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="847" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="847" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B847" s="2" t="s">
         <v>59</v>
       </c>
@@ -15076,7 +15165,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="848" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="848" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B848" s="2" t="s">
         <v>59</v>
       </c>
@@ -15383,7 +15472,7 @@
       <c r="E869" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G869" s="2" t="s">
+      <c r="G869" s="14" t="s">
         <v>61</v>
       </c>
     </row>
@@ -15778,7 +15867,7 @@
       <c r="E897" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G897" s="2" t="s">
+      <c r="G897" s="14" t="s">
         <v>62</v>
       </c>
     </row>
@@ -15795,7 +15884,7 @@
       <c r="E898" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G898" s="2" t="s">
+      <c r="G898" s="14" t="s">
         <v>62</v>
       </c>
     </row>
@@ -15995,7 +16084,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="913" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="913" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B913" s="2" t="s">
         <v>59</v>
       </c>
@@ -16009,7 +16098,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="914" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="914" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B914" s="2" t="s">
         <v>59</v>
       </c>
@@ -16023,7 +16112,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="915" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="915" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B915" s="2" t="s">
         <v>59</v>
       </c>
@@ -16037,7 +16126,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="916" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="916" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B916" s="2" t="s">
         <v>59</v>
       </c>
@@ -16051,7 +16140,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="917" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="917" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B917" s="2" t="s">
         <v>59</v>
       </c>
@@ -16065,7 +16154,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="918" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="918" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B918" s="2" t="s">
         <v>59</v>
       </c>
@@ -16079,7 +16168,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="919" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="919" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B919" s="2" t="s">
         <v>59</v>
       </c>
@@ -16093,7 +16182,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="920" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="920" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B920" s="2" t="s">
         <v>59</v>
       </c>
@@ -16107,7 +16196,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="921" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="921" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B921" s="2" t="s">
         <v>59</v>
       </c>
@@ -16121,7 +16210,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="922" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="922" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B922" s="2" t="s">
         <v>59</v>
       </c>
@@ -16135,7 +16224,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="923" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="923" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B923" s="2" t="s">
         <v>84</v>
       </c>
@@ -16146,7 +16235,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="924" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="924" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B924" s="2" t="s">
         <v>84</v>
       </c>
@@ -16160,7 +16249,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="925" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="925" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B925" s="2" t="s">
         <v>84</v>
       </c>
@@ -16174,7 +16263,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="926" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="926" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B926" s="2" t="s">
         <v>84</v>
       </c>
@@ -16188,7 +16277,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="927" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="927" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B927" s="2" t="s">
         <v>84</v>
       </c>
@@ -16204,11 +16293,14 @@
       <c r="F927" s="2">
         <v>3</v>
       </c>
-      <c r="G927" s="2" t="s">
+      <c r="G927" s="14" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="928" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H927" s="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="928" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B928" s="2" t="s">
         <v>84</v>
       </c>
@@ -16446,7 +16538,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="945" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="945" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B945" s="2" t="s">
         <v>84</v>
       </c>
@@ -16460,7 +16552,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="946" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="946" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B946" s="2" t="s">
         <v>84</v>
       </c>
@@ -16474,7 +16566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="947" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="947" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B947" s="2" t="s">
         <v>84</v>
       </c>
@@ -16490,11 +16582,14 @@
       <c r="F947" s="2">
         <v>4</v>
       </c>
-      <c r="G947" s="2" t="s">
+      <c r="G947" s="14" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="948" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H947" s="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="948" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B948" s="2" t="s">
         <v>84</v>
       </c>
@@ -16507,11 +16602,14 @@
       <c r="E948" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G948" s="2" t="s">
+      <c r="G948" s="14" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="949" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H948">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="949" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B949" s="2" t="s">
         <v>84</v>
       </c>
@@ -16524,11 +16622,14 @@
       <c r="E949" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G949" s="2" t="s">
+      <c r="G949" s="14" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="950" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H949">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="950" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B950" s="2" t="s">
         <v>84</v>
       </c>
@@ -16542,7 +16643,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="951" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="951" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B951" s="2" t="s">
         <v>84</v>
       </c>
@@ -16558,11 +16659,14 @@
       <c r="F951" s="2">
         <v>3</v>
       </c>
-      <c r="G951" s="2" t="s">
+      <c r="G951" s="14" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="952" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H951" s="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="952" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B952" s="2" t="s">
         <v>84</v>
       </c>
@@ -16576,7 +16680,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="953" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="953" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B953" s="2" t="s">
         <v>84</v>
       </c>
@@ -16590,7 +16694,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="954" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="954" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B954" s="2" t="s">
         <v>84</v>
       </c>
@@ -16604,7 +16708,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="955" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="955" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B955" s="2" t="s">
         <v>84</v>
       </c>
@@ -16618,7 +16722,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="956" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="956" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B956" s="2" t="s">
         <v>84</v>
       </c>
@@ -16632,7 +16736,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="957" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="957" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B957" s="2" t="s">
         <v>84</v>
       </c>
@@ -16648,8 +16752,11 @@
       <c r="F957" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="958" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H957" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="958" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B958" s="2" t="s">
         <v>84</v>
       </c>
@@ -16663,7 +16770,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="959" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="959" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B959" s="2" t="s">
         <v>84</v>
       </c>
@@ -16677,7 +16784,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="960" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="960" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B960" s="2" t="s">
         <v>84</v>
       </c>
@@ -16691,7 +16798,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="961" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="961" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B961" s="2" t="s">
         <v>84</v>
       </c>
@@ -16705,7 +16812,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="962" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="962" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B962" s="2" t="s">
         <v>84</v>
       </c>
@@ -16719,7 +16826,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="963" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="963" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B963" s="2" t="s">
         <v>84</v>
       </c>
@@ -16733,7 +16840,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="964" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="964" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B964" s="2" t="s">
         <v>84</v>
       </c>
@@ -16747,7 +16854,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="965" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="965" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B965" s="2" t="s">
         <v>84</v>
       </c>
@@ -16761,18 +16868,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="966" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="966" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B966" s="2" t="s">
         <v>84</v>
       </c>
       <c r="D966" s="2">
         <v>144</v>
       </c>
-      <c r="G966" s="2" t="s">
+      <c r="G966" s="14" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="967" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H966">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="967" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B967" s="2" t="s">
         <v>84</v>
       </c>
@@ -16786,7 +16896,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="968" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="968" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B968" s="2" t="s">
         <v>84</v>
       </c>
@@ -16800,7 +16910,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="969" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="969" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B969" s="2" t="s">
         <v>84</v>
       </c>
@@ -16814,7 +16924,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="970" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="970" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B970" s="2" t="s">
         <v>84</v>
       </c>
@@ -16828,7 +16938,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="971" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="971" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B971" s="2" t="s">
         <v>84</v>
       </c>
@@ -16842,7 +16952,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="972" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="972" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B972" s="2" t="s">
         <v>84</v>
       </c>
@@ -16856,7 +16966,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="973" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="973" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B973" s="2" t="s">
         <v>84</v>
       </c>
@@ -16870,7 +16980,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="974" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="974" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B974" s="2" t="s">
         <v>84</v>
       </c>
@@ -16884,7 +16994,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="975" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="975" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B975" s="2" t="s">
         <v>84</v>
       </c>
@@ -16898,7 +17008,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="976" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="976" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B976" s="2" t="s">
         <v>84</v>
       </c>
@@ -16912,7 +17022,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="977" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="977" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B977" s="2" t="s">
         <v>84</v>
       </c>
@@ -16926,7 +17036,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="978" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="978" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B978" s="2" t="s">
         <v>84</v>
       </c>
@@ -16940,7 +17050,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="979" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="979" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B979" s="2" t="s">
         <v>84</v>
       </c>
@@ -16954,7 +17064,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="980" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="980" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B980" s="2" t="s">
         <v>84</v>
       </c>
@@ -16968,7 +17078,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="981" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="981" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B981" s="2" t="s">
         <v>84</v>
       </c>
@@ -16982,7 +17092,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="982" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="982" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B982" s="2" t="s">
         <v>84</v>
       </c>
@@ -16996,7 +17106,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="983" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="983" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B983" s="2" t="s">
         <v>84</v>
       </c>
@@ -17010,7 +17120,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="984" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="984" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B984" s="2" t="s">
         <v>84</v>
       </c>
@@ -17026,11 +17136,14 @@
       <c r="F984" s="2">
         <v>3</v>
       </c>
-      <c r="G984" s="2" t="s">
+      <c r="G984" s="14" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="985" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H984" s="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="985" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B985" s="2" t="s">
         <v>84</v>
       </c>
@@ -17044,7 +17157,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="986" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="986" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B986" s="2" t="s">
         <v>84</v>
       </c>
@@ -17060,8 +17173,11 @@
       <c r="F986" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="987" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H986" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="987" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B987" s="2" t="s">
         <v>84</v>
       </c>
@@ -17075,7 +17191,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="988" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="988" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B988" s="2" t="s">
         <v>84</v>
       </c>
@@ -17089,7 +17205,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="989" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="989" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B989" s="2" t="s">
         <v>84</v>
       </c>
@@ -17103,7 +17219,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="990" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="990" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B990" s="2" t="s">
         <v>84</v>
       </c>
@@ -17117,7 +17233,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="991" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="991" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B991" s="2" t="s">
         <v>84</v>
       </c>
@@ -17131,7 +17247,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="992" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="992" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B992" s="2" t="s">
         <v>84</v>
       </c>
@@ -17158,7 +17274,7 @@
         <v>41</v>
       </c>
       <c r="F993" s="6"/>
-      <c r="G993" s="6"/>
+      <c r="G993" s="13"/>
     </row>
     <row r="994" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B994" s="2" t="s">
@@ -18490,7 +18606,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="1089" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1089" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1089" s="2" t="s">
         <v>89</v>
       </c>
@@ -18504,7 +18620,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="1090" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1090" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1090" s="2" t="s">
         <v>89</v>
       </c>
@@ -18518,7 +18634,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="1091" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1091" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1091" s="2" t="s">
         <v>89</v>
       </c>
@@ -18532,7 +18648,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="1092" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1092" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1092" s="2" t="s">
         <v>89</v>
       </c>
@@ -18546,7 +18662,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="1093" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1093" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1093" s="2" t="s">
         <v>89</v>
       </c>
@@ -18560,7 +18676,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="1094" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1094" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1094" s="2" t="s">
         <v>89</v>
       </c>
@@ -18574,7 +18690,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="1095" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1095" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1095" s="2" t="s">
         <v>89</v>
       </c>
@@ -18588,7 +18704,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="1096" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1096" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1096" s="2" t="s">
         <v>89</v>
       </c>
@@ -18601,11 +18717,11 @@
       <c r="E1096" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G1096" s="2" t="s">
+      <c r="G1096" s="14" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="1097" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1097" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1097" s="2" t="s">
         <v>89</v>
       </c>
@@ -18618,11 +18734,11 @@
       <c r="E1097" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G1097" s="2" t="s">
+      <c r="G1097" s="14" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="1098" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1098" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1098" s="2" t="s">
         <v>89</v>
       </c>
@@ -18636,7 +18752,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="1099" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1099" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1099" s="2" t="s">
         <v>89</v>
       </c>
@@ -18650,7 +18766,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="1100" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1100" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1100" s="2" t="s">
         <v>89</v>
       </c>
@@ -18664,7 +18780,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="1101" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1101" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1101" s="2" t="s">
         <v>89</v>
       </c>
@@ -18678,7 +18794,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="1102" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1102" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1102" s="2" t="s">
         <v>89</v>
       </c>
@@ -18692,7 +18808,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="1103" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1103" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1103" s="2" t="s">
         <v>89</v>
       </c>
@@ -18706,7 +18822,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="1104" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1104" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1104" s="2" t="s">
         <v>89</v>
       </c>
@@ -18719,11 +18835,14 @@
       <c r="E1104" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G1104" s="2" t="s">
+      <c r="G1104" s="14" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="1105" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H1104">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1105" s="2" t="s">
         <v>89</v>
       </c>
@@ -18736,11 +18855,14 @@
       <c r="E1105" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G1105" s="2" t="s">
+      <c r="G1105" s="14" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="1106" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H1105">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1106" s="2" t="s">
         <v>89</v>
       </c>
@@ -18754,7 +18876,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="1107" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1107" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1107" s="2" t="s">
         <v>89</v>
       </c>
@@ -18768,7 +18890,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="1108" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1108" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1108" s="2" t="s">
         <v>89</v>
       </c>
@@ -18782,7 +18904,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="1109" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1109" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1109" s="2" t="s">
         <v>89</v>
       </c>
@@ -18796,7 +18918,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="1110" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1110" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1110" s="2" t="s">
         <v>89</v>
       </c>
@@ -18810,7 +18932,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="1111" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1111" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1111" s="2" t="s">
         <v>89</v>
       </c>
@@ -18824,7 +18946,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="1112" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1112" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1112" s="2" t="s">
         <v>89</v>
       </c>
@@ -18837,11 +18959,14 @@
       <c r="E1112" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G1112" s="2" t="s">
+      <c r="G1112" s="14" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="1113" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H1112">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1113" s="2" t="s">
         <v>89</v>
       </c>
@@ -18854,11 +18979,14 @@
       <c r="E1113" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G1113" s="2" t="s">
+      <c r="G1113" s="14" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="1114" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H1113">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A1114" s="6"/>
       <c r="B1114" s="6" t="s">
         <v>89</v>
@@ -18871,9 +18999,9 @@
         <v>41</v>
       </c>
       <c r="F1114" s="6"/>
-      <c r="G1114" s="6"/>
-    </row>
-    <row r="1115" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="G1114" s="13"/>
+    </row>
+    <row r="1115" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1115" s="2" t="s">
         <v>76</v>
       </c>
@@ -18884,7 +19012,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="1116" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1116" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1116" s="2" t="s">
         <v>76</v>
       </c>
@@ -18898,7 +19026,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="1117" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1117" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1117" s="2" t="s">
         <v>76</v>
       </c>
@@ -18912,7 +19040,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="1118" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1118" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1118" s="2" t="s">
         <v>76</v>
       </c>
@@ -18926,7 +19054,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="1119" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1119" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1119" s="2" t="s">
         <v>76</v>
       </c>
@@ -18940,7 +19068,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="1120" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1120" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1120" s="2" t="s">
         <v>76</v>
       </c>
@@ -20295,7 +20423,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="1217" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1217" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1217" s="2" t="s">
         <v>85</v>
       </c>
@@ -20309,7 +20437,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="1218" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1218" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1218" s="2" t="s">
         <v>85</v>
       </c>
@@ -20325,11 +20453,14 @@
       <c r="F1218" s="2">
         <v>2</v>
       </c>
-      <c r="G1218" s="2" t="s">
+      <c r="G1218" s="14" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="1219" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H1218" s="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1219" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1219" s="2" t="s">
         <v>85</v>
       </c>
@@ -20343,7 +20474,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="1220" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1220" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1220" s="2" t="s">
         <v>85</v>
       </c>
@@ -20359,11 +20490,14 @@
       <c r="F1220" s="2">
         <v>2</v>
       </c>
-      <c r="G1220" s="2" t="s">
+      <c r="G1220" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="1221" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H1220" s="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1221" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1221" s="2" t="s">
         <v>85</v>
       </c>
@@ -20377,7 +20511,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="1222" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1222" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1222" s="2" t="s">
         <v>85</v>
       </c>
@@ -20393,8 +20527,11 @@
       <c r="F1222" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="1223" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H1222" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1223" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1223" s="2" t="s">
         <v>85</v>
       </c>
@@ -20408,7 +20545,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="1224" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1224" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1224" s="2" t="s">
         <v>85</v>
       </c>
@@ -20422,7 +20559,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="1225" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1225" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1225" s="2" t="s">
         <v>85</v>
       </c>
@@ -20436,7 +20573,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="1226" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1226" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1226" s="2" t="s">
         <v>85</v>
       </c>
@@ -20450,7 +20587,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="1227" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1227" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1227" s="2" t="s">
         <v>85</v>
       </c>
@@ -20464,7 +20601,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="1228" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1228" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1228" s="2" t="s">
         <v>85</v>
       </c>
@@ -20478,7 +20615,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="1229" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1229" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1229" s="2" t="s">
         <v>85</v>
       </c>
@@ -20492,7 +20629,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="1230" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1230" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1230" s="2" t="s">
         <v>85</v>
       </c>
@@ -20506,7 +20643,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="1231" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1231" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1231" s="2" t="s">
         <v>85</v>
       </c>
@@ -20520,7 +20657,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="1232" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1232" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1232" s="2" t="s">
         <v>85</v>
       </c>
@@ -20659,7 +20796,7 @@
       <c r="E1241" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1241" s="2" t="s">
+      <c r="G1241" s="14" t="s">
         <v>79</v>
       </c>
     </row>
@@ -20761,7 +20898,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="1249" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1249" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1249" s="2" t="s">
         <v>85</v>
       </c>
@@ -20775,7 +20912,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="1250" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1250" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1250" s="2" t="s">
         <v>85</v>
       </c>
@@ -20789,7 +20926,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="1251" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1251" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1251" s="2" t="s">
         <v>85</v>
       </c>
@@ -20803,7 +20940,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="1252" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1252" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1252" s="2" t="s">
         <v>85</v>
       </c>
@@ -20817,7 +20954,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="1253" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1253" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1253" s="2" t="s">
         <v>85</v>
       </c>
@@ -20830,11 +20967,11 @@
       <c r="E1253" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1253" s="2" t="s">
+      <c r="G1253" s="14" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="1254" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1254" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1254" s="2" t="s">
         <v>85</v>
       </c>
@@ -20848,7 +20985,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="1255" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1255" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1255" s="2" t="s">
         <v>85</v>
       </c>
@@ -20862,7 +20999,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="1256" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1256" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1256" s="2" t="s">
         <v>85</v>
       </c>
@@ -20876,7 +21013,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="1257" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1257" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1257" s="2" t="s">
         <v>85</v>
       </c>
@@ -20890,7 +21027,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="1258" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1258" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1258" s="2" t="s">
         <v>85</v>
       </c>
@@ -20904,7 +21041,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="1259" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1259" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1259" s="2" t="s">
         <v>85</v>
       </c>
@@ -20918,7 +21055,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="1260" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1260" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1260" s="2" t="s">
         <v>85</v>
       </c>
@@ -20931,11 +21068,14 @@
       <c r="E1260" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1260" s="2" t="s">
+      <c r="G1260" s="14" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="1261" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H1260">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1261" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1261" s="2" t="s">
         <v>85</v>
       </c>
@@ -20949,7 +21089,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="1262" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1262" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1262" s="2" t="s">
         <v>85</v>
       </c>
@@ -20963,7 +21103,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1263" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1263" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1263" s="2" t="s">
         <v>85</v>
       </c>
@@ -20977,7 +21117,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="1264" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1264" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1264" s="2" t="s">
         <v>85</v>
       </c>
@@ -21215,7 +21355,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="1281" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1281" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1281" s="2" t="s">
         <v>85</v>
       </c>
@@ -21229,7 +21369,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="1282" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1282" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1282" s="2" t="s">
         <v>85</v>
       </c>
@@ -21243,7 +21383,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="1283" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1283" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1283" s="2" t="s">
         <v>85</v>
       </c>
@@ -21257,7 +21397,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="1284" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1284" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1284" s="2" t="s">
         <v>85</v>
       </c>
@@ -21271,7 +21411,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="1285" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1285" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1285" s="2" t="s">
         <v>85</v>
       </c>
@@ -21285,7 +21425,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="1286" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1286" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1286" s="2" t="s">
         <v>85</v>
       </c>
@@ -21299,7 +21439,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="1287" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1287" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1287" s="2" t="s">
         <v>85</v>
       </c>
@@ -21313,7 +21453,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="1288" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1288" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1288" s="2" t="s">
         <v>85</v>
       </c>
@@ -21327,7 +21467,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="1289" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1289" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1289" s="2" t="s">
         <v>85</v>
       </c>
@@ -21341,7 +21481,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="1290" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1290" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1290" s="2" t="s">
         <v>85</v>
       </c>
@@ -21355,51 +21495,63 @@
         <v>32</v>
       </c>
     </row>
-    <row r="1291" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1291" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1291" s="2" t="s">
         <v>85</v>
       </c>
       <c r="D1291" s="2">
         <v>200</v>
       </c>
-      <c r="G1291" s="2" t="s">
+      <c r="G1291" s="14" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="1292" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H1291">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1292" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1292" s="2" t="s">
         <v>85</v>
       </c>
       <c r="D1292" s="2">
         <v>201</v>
       </c>
-      <c r="G1292" s="2" t="s">
+      <c r="G1292" s="14" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="1293" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H1292">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1293" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1293" s="2" t="s">
         <v>85</v>
       </c>
       <c r="D1293" s="2">
         <v>202</v>
       </c>
-      <c r="G1293" s="2" t="s">
+      <c r="G1293" s="14" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="1294" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H1293">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1294" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1294" s="2" t="s">
         <v>85</v>
       </c>
       <c r="D1294" s="2">
         <v>203</v>
       </c>
-      <c r="G1294" s="2" t="s">
+      <c r="G1294" s="14" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="1295" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H1294">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1295" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1295" s="2" t="s">
         <v>85</v>
       </c>
@@ -21413,7 +21565,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="1296" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1296" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1296" s="2" t="s">
         <v>85</v>
       </c>
@@ -21563,7 +21715,7 @@
         <v>45</v>
       </c>
       <c r="F1306" s="10"/>
-      <c r="G1306" s="10"/>
+      <c r="G1306" s="17"/>
       <c r="H1306" s="10"/>
       <c r="I1306" s="10"/>
       <c r="J1306" s="10"/>
@@ -21671,7 +21823,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="1313" spans="2:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1313" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1313" s="2" t="s">
         <v>90</v>
       </c>
@@ -21685,7 +21837,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="1314" spans="2:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1314" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1314" s="2" t="s">
         <v>90</v>
       </c>
@@ -21699,7 +21851,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="1315" spans="2:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1315" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1315" s="2" t="s">
         <v>90</v>
       </c>
@@ -21713,7 +21865,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="1316" spans="2:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1316" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1316" s="2" t="s">
         <v>90</v>
       </c>
@@ -21727,7 +21879,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="1317" spans="2:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1317" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1317" s="2" t="s">
         <v>90</v>
       </c>
@@ -21737,8 +21889,11 @@
       <c r="F1317" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="1318" spans="2:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H1317">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1318" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1318" s="2" t="s">
         <v>90</v>
       </c>
@@ -21748,8 +21903,11 @@
       <c r="F1318" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="1319" spans="2:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H1318">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1319" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1319" s="2" t="s">
         <v>90</v>
       </c>
@@ -21763,7 +21921,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="1320" spans="2:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1320" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1320" s="2" t="s">
         <v>90</v>
       </c>
@@ -21777,7 +21935,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="1321" spans="2:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1321" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1321" s="2" t="s">
         <v>90</v>
       </c>
@@ -21791,7 +21949,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="1322" spans="2:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1322" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1322" s="2" t="s">
         <v>90</v>
       </c>
@@ -21805,7 +21963,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="1323" spans="2:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1323" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1323" s="2" t="s">
         <v>90</v>
       </c>
@@ -21819,7 +21977,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="1324" spans="2:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1324" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1324" s="2" t="s">
         <v>90</v>
       </c>
@@ -21833,7 +21991,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="1325" spans="2:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1325" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1325" s="2" t="s">
         <v>90</v>
       </c>
@@ -21847,7 +22005,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="1326" spans="2:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1326" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1326" s="2" t="s">
         <v>90</v>
       </c>
@@ -21861,7 +22019,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="1327" spans="2:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1327" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1327" s="2" t="s">
         <v>90</v>
       </c>
@@ -21875,7 +22033,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="1328" spans="2:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1328" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B1328" s="2" t="s">
         <v>90</v>
       </c>
@@ -22294,7 +22452,7 @@
       <c r="E1357" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G1357" s="2" t="s">
+      <c r="G1357" s="14" t="s">
         <v>81</v>
       </c>
     </row>
@@ -22632,7 +22790,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AC1381" xr:uid="{72D9BBEF-D41B-3943-88E3-081E080D25A5}"/>
   <mergeCells count="1">
     <mergeCell ref="G109:G110"/>
   </mergeCells>

</xml_diff>